<commit_message>
IMPORT FILE MTC ADJUST
</commit_message>
<xml_diff>
--- a/public/assets/EmployeeImport.xlsx
+++ b/public/assets/EmployeeImport.xlsx
@@ -25,73 +25,73 @@
     <t xml:space="preserve">NIK</t>
   </si>
   <si>
-    <t xml:space="preserve">Name</t>
+    <t xml:space="preserve">NAME</t>
   </si>
   <si>
     <t xml:space="preserve">KTP</t>
   </si>
   <si>
-    <t xml:space="preserve">Phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timezone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rekening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Join Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subarea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales Tier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timezone Store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Education</t>
+    <t xml:space="preserve">PHONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIMEZONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REKENING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOIN DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENCY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIRTH DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBAREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCOUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHANNEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASSWORD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SALES TIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIMEZONE STORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATION</t>
   </si>
   <si>
     <t xml:space="preserve">13111</t>
@@ -168,7 +168,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -270,6 +270,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -427,12 +435,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -543,8 +559,8 @@
   </sheetPr>
   <dimension ref="A1:Y65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y1" activeCellId="0" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -553,7 +569,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -626,58 +642,58 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="R2" s="0" t="s">
@@ -698,7 +714,7 @@
       <c r="W2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="4" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update excell file import template employee mtc
</commit_message>
<xml_diff>
--- a/public/assets/EmployeeImport.xlsx
+++ b/public/assets/EmployeeImport.xlsx
@@ -559,8 +559,8 @@
   </sheetPr>
   <dimension ref="A1:Y65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y1" activeCellId="0" sqref="Y1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>